<commit_message>
Update to CDM online manual Appendix B
</commit_message>
<xml_diff>
--- a/docs/CDM-manual/tables/CIIP_phase2_scenarios.xlsx
+++ b/docs/CDM-manual/tables/CIIP_phase2_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\docs\CDM-manual\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD7132A-AD2E-4E0B-BCB5-EF44DF064531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AFD1C3-DDCA-490D-9FC7-4582FD682676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9975" yWindow="2985" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5055" yWindow="2490" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="56">
   <si>
     <t>OXY</t>
   </si>
@@ -112,23 +112,89 @@
     <t>Dark</t>
   </si>
   <si>
-    <t>~250</t>
-  </si>
-  <si>
-    <t>~160</t>
-  </si>
-  <si>
-    <t>455 ± 286</t>
-  </si>
-  <si>
     <t>28.3 ± 16.9</t>
   </si>
   <si>
     <t>1546 ± 2857</t>
   </si>
   <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>mmol m-2 d-1</t>
+  </si>
+  <si>
+    <t>umol m-2 h-1</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Zone 1</t>
+  </si>
+  <si>
+    <t>Zone 2</t>
+  </si>
+  <si>
+    <t>Zone 3</t>
+  </si>
+  <si>
+    <t>Zone 4</t>
+  </si>
+  <si>
+    <t>Zone 5</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>253 ± 88.4</t>
+  </si>
+  <si>
+    <t>172.5 ± 107.6</t>
+  </si>
+  <si>
+    <t>6.07 ± 2.12</t>
+  </si>
+  <si>
+    <t>4.14 ± 2.58</t>
+  </si>
+  <si>
+    <t>267.2 ± 269.8</t>
+  </si>
+  <si>
+    <t>2.90 ± 43.6</t>
+  </si>
+  <si>
+    <t>6.41 ± 6.47</t>
+  </si>
+  <si>
+    <t>0.07 ± 1.05</t>
+  </si>
+  <si>
+    <t>5.6 ± 5.8</t>
+  </si>
+  <si>
+    <t>0.13 ± 0.14</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">4925 ± 541 </t>
+      <t xml:space="preserve">-4925 ± 541 </t>
     </r>
     <r>
       <rPr>
@@ -142,49 +208,13 @@
     </r>
   </si>
   <si>
-    <t>Raw</t>
-  </si>
-  <si>
-    <t>AED</t>
-  </si>
-  <si>
-    <t>mmol m-2 d-1</t>
-  </si>
-  <si>
-    <t>umol m-2 h-1</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Zone 1</t>
-  </si>
-  <si>
-    <t>Zone 2</t>
-  </si>
-  <si>
-    <t>Zone 3</t>
-  </si>
-  <si>
-    <t>Zone 4</t>
-  </si>
-  <si>
-    <t>Zone 5</t>
-  </si>
-  <si>
-    <t>Scenario</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Dataset</t>
-  </si>
-  <si>
-    <t>Units</t>
+    <t>37.1 ± 68.57</t>
+  </si>
+  <si>
+    <t>-118.2  ± 12.98</t>
+  </si>
+  <si>
+    <t>0.68 ± 0.41</t>
   </si>
 </sst>
 </file>
@@ -267,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,6 +316,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,28 +611,28 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -620,7 +652,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>12</v>
@@ -661,7 +693,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>12</v>
@@ -702,7 +734,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>12</v>
@@ -743,7 +775,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>12</v>
@@ -784,7 +816,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>12</v>
@@ -825,7 +857,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>13</v>
@@ -851,7 +883,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>13</v>
@@ -877,7 +909,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>13</v>
@@ -903,7 +935,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>13</v>
@@ -929,7 +961,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>13</v>
@@ -955,7 +987,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>14</v>
@@ -981,7 +1013,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>14</v>
@@ -1007,7 +1039,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>14</v>
@@ -1033,7 +1065,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>14</v>
@@ -1059,7 +1091,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>14</v>
@@ -1085,7 +1117,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>15</v>
@@ -1111,7 +1143,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>15</v>
@@ -1137,7 +1169,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>15</v>
@@ -1163,7 +1195,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>15</v>
@@ -1189,7 +1221,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>15</v>
@@ -1409,7 +1441,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,16 +1451,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>23</v>
@@ -1439,168 +1471,162 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="2">
-        <f>250*24/1000</f>
-        <v>6</v>
-      </c>
-      <c r="F3" s="5">
-        <f>160*24/1000</f>
-        <v>3.84</v>
+        <v>29</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="2">
-        <f>455*24/1000</f>
-        <v>10.92</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <f>28.3*24/1000</f>
-        <v>0.67920000000000003</v>
+        <v>29</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="5" t="s">
         <v>30</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="2">
-        <f>1546*24/1000</f>
-        <v>37.103999999999999</v>
-      </c>
-      <c r="F9" s="5">
-        <f>4925*24/1000</f>
-        <v>118.2</v>
+        <v>29</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>